<commit_message>
DB_Memory: Updated all files with the new description of 0 ohms jumper resistor (before with 1/16W now with 1/8W)
</commit_message>
<xml_diff>
--- a/Memory_Expansion_Daughter_Board/hardware/Output_files/Bill of Materials/Bill of Materials-DB_Memory.xlsx
+++ b/Memory_Expansion_Daughter_Board/hardware/Output_files/Bill of Materials/Bill of Materials-DB_Memory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{126D8BD8-2422-43CB-BB99-CF544DB7A9EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B074A4F-AD01-4C72-9C6D-F0583FEA357B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1605" yWindow="1605" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
     <t>24/03/2020</t>
   </si>
   <si>
-    <t>00:35:22</t>
+    <t>11:18:38</t>
   </si>
   <si>
     <t>Supplier 1</t>
@@ -271,7 +271,7 @@
     <t>Fiducial for DB board variants</t>
   </si>
   <si>
-    <t>RES 0R OHM 1/16W JUMPER 0805</t>
+    <t>RES 0R OHM 1/8W JUMPER 0805</t>
   </si>
   <si>
     <t>Conn Unshrouded Header HDR 3 POS 2.54mm Solder RA Thru-Hole Automotive Bulk</t>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="H8" s="16">
         <f ca="1">NOW()</f>
-        <v>43914.024709375</v>
+        <v>43914.471456712963</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
@@ -2104,38 +2104,38 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" tooltip="Supplier" display="'541-10.0KCCT-ND" xr:uid="{3CB880F1-17B5-4EF6-A406-46BE4AF0688F}"/>
-    <hyperlink ref="C12" tooltip="Supplier" display="'" xr:uid="{4AB6F885-2549-49C4-89FE-00489F3A2F82}"/>
-    <hyperlink ref="C13" tooltip="Supplier" display="'" xr:uid="{7EFA4D85-DC66-48D6-9038-75EC4D89033F}"/>
-    <hyperlink ref="C14" r:id="rId2" tooltip="Supplier" display="'311-0.0ARCT-ND" xr:uid="{277E53C0-CF03-43D2-B7F8-4BB0A246CB90}"/>
-    <hyperlink ref="C15" r:id="rId3" tooltip="Supplier" display="'200-TSW10308GSRA" xr:uid="{4993F103-A141-4AB2-AE2A-DC0600CFA9E0}"/>
-    <hyperlink ref="C16" r:id="rId4" tooltip="Supplier" display="'160-1413-1-ND" xr:uid="{E2C7AA09-616B-4D8E-A3FF-2CF2FFA9CA55}"/>
-    <hyperlink ref="C17" r:id="rId5" tooltip="Supplier" display="'296-1222-1-ND" xr:uid="{694BE194-F082-49FD-9AD5-8653B31FDF25}"/>
-    <hyperlink ref="C18" r:id="rId6" tooltip="Supplier" display="'311-100KCRCT-ND" xr:uid="{1D35770D-2B0F-4968-994C-EB25F196EB7D}"/>
-    <hyperlink ref="C19" r:id="rId7" tooltip="Supplier" display="'311-1141-1-ND" xr:uid="{CF99A6DB-CD96-4160-AE04-0926A80E7D9B}"/>
-    <hyperlink ref="C20" r:id="rId8" tooltip="Supplier" display="'311-1401-1-ND" xr:uid="{E9BCE6FE-0120-499C-84F7-2A2C9FADD276}"/>
-    <hyperlink ref="C21" r:id="rId9" tooltip="Supplier" display="'587-2990-6-ND" xr:uid="{EDA7DECF-E6BF-4603-9E7D-BC37F3B1B1F4}"/>
-    <hyperlink ref="C22" r:id="rId10" tooltip="Supplier" display="'2019-RK73H2ATTD3300FCT-ND" xr:uid="{11DAC731-9C8F-4387-AE94-31D9DC1AE4CF}"/>
-    <hyperlink ref="C23" r:id="rId11" tooltip="Supplier" display="'200-FSI11003GDAD" xr:uid="{79A6DE26-D84B-499E-9477-162A949EACA1}"/>
-    <hyperlink ref="C24" r:id="rId12" tooltip="Supplier" display="'200-TSW10208GSRA" xr:uid="{8D76C9FD-C82B-4A48-826E-3D11376F63D4}"/>
-    <hyperlink ref="C25" r:id="rId13" tooltip="Supplier" display="'340-278808-TRAY" xr:uid="{63880A94-11F5-48F1-A20F-C2CD6C740402}"/>
-    <hyperlink ref="C26" r:id="rId14" tooltip="Supplier" display="'538-503182-1852" xr:uid="{5FEADB25-3796-487A-9F8E-E329E760D8AB}"/>
-    <hyperlink ref="E11" r:id="rId15" tooltip="Supplier" display="'71-CRCW0805-10K-E3" xr:uid="{847C21E9-BE2A-46BA-8584-769F485C8791}"/>
-    <hyperlink ref="E12" tooltip="Supplier" display="'" xr:uid="{4EE9867F-052F-4A72-A50E-6C8436AF88CE}"/>
-    <hyperlink ref="E13" tooltip="Supplier" display="'" xr:uid="{CC415C66-F002-42CE-AC0C-CDDD8D3CA946}"/>
-    <hyperlink ref="E14" r:id="rId16" tooltip="Supplier" display="'603-RC0805JR-070RL" xr:uid="{23895821-CAC7-49F6-A027-7888A689F7CC}"/>
-    <hyperlink ref="E15" r:id="rId17" tooltip="Supplier" display="'SAM1039-03-ND" xr:uid="{EB1E48B6-B89D-4972-812B-17E5061D3D27}"/>
-    <hyperlink ref="E16" r:id="rId18" tooltip="Supplier" display="'859-LTST-C170KFKT" xr:uid="{FEEE4163-1CD6-4267-81AE-FA3523B1C040}"/>
-    <hyperlink ref="E17" r:id="rId19" tooltip="Supplier" display="'595-SN74LVC125APWR" xr:uid="{2993C8B4-344B-45A4-8EED-A4E494EB18E3}"/>
-    <hyperlink ref="E18" r:id="rId20" tooltip="Supplier" display="'603-RC0805FR-07100KL" xr:uid="{922702F0-B984-40C7-8DDB-C5B676389EF5}"/>
-    <hyperlink ref="E19" r:id="rId21" tooltip="Supplier" display="'603-CC805KRX7R8BB104" xr:uid="{A886F637-052E-4054-9D29-800492BA9B3A}"/>
-    <hyperlink ref="E20" r:id="rId22" tooltip="Supplier" display="'603-CC201KRX7R9BB101" xr:uid="{D6B0FAC8-5AF7-4A45-AE0D-F9393CEDA2D8}"/>
-    <hyperlink ref="E21" r:id="rId23" tooltip="Supplier" display="'963-TMK212AB7475KG-T" xr:uid="{98D46D76-3523-4817-97F3-FBE67A086603}"/>
-    <hyperlink ref="E22" r:id="rId24" tooltip="Supplier" display="'660-RK73H2ATTD3300F" xr:uid="{FD096F9D-133F-4329-88A9-E37A66627CC5}"/>
-    <hyperlink ref="E23" r:id="rId25" tooltip="Supplier" display="'SAM9412-ND" xr:uid="{2F2387A6-C9F8-4954-B05E-C1E517DFD0CF}"/>
-    <hyperlink ref="E24" r:id="rId26" tooltip="Supplier" display="'SAM1039-02-ND" xr:uid="{5DF4C881-C282-49D9-85F8-25EC6DB5CB1A}"/>
-    <hyperlink ref="E25" r:id="rId27" tooltip="Supplier" display="'557-1789-ND" xr:uid="{A87BC914-F8B1-4EE8-B8C4-CF29261FD5D7}"/>
-    <hyperlink ref="E26" r:id="rId28" tooltip="Supplier" display="'WM12834CT-ND" xr:uid="{12CBDC1E-D067-44D3-B303-AB631ABEBDBD}"/>
+    <hyperlink ref="C11" r:id="rId1" tooltip="Supplier" display="'541-10.0KCCT-ND" xr:uid="{EDD08F27-801C-46DA-8E9F-C88562AF06A0}"/>
+    <hyperlink ref="C12" tooltip="Supplier" display="'" xr:uid="{390C8A83-7557-43B3-8AF5-B4D02F0E7959}"/>
+    <hyperlink ref="C13" tooltip="Supplier" display="'" xr:uid="{C5523B0D-FD17-4283-A930-B677E2FE27ED}"/>
+    <hyperlink ref="C14" r:id="rId2" tooltip="Supplier" display="'311-0.0ARCT-ND" xr:uid="{7F3F3DB4-E824-4A2C-A891-52D00F4D7ACC}"/>
+    <hyperlink ref="C15" r:id="rId3" tooltip="Supplier" display="'200-TSW10308GSRA" xr:uid="{D7A61844-0204-42C8-91B5-D5F4C3CEC40E}"/>
+    <hyperlink ref="C16" r:id="rId4" tooltip="Supplier" display="'160-1413-1-ND" xr:uid="{AC6E6377-A61E-4DD5-B45A-B8CE4BCD27DD}"/>
+    <hyperlink ref="C17" r:id="rId5" tooltip="Supplier" display="'296-1222-1-ND" xr:uid="{6CBB4872-E5BA-4F10-B373-DE1DB3D918A4}"/>
+    <hyperlink ref="C18" r:id="rId6" tooltip="Supplier" display="'311-100KCRCT-ND" xr:uid="{70AFAAAD-37F8-475F-8E70-BDF4AB2D6FDA}"/>
+    <hyperlink ref="C19" r:id="rId7" tooltip="Supplier" display="'311-1141-1-ND" xr:uid="{E5CC9A02-8005-4EB3-9174-4019B579B0DA}"/>
+    <hyperlink ref="C20" r:id="rId8" tooltip="Supplier" display="'311-1401-1-ND" xr:uid="{0B343FEF-8427-483E-B423-D63E825B98CE}"/>
+    <hyperlink ref="C21" r:id="rId9" tooltip="Supplier" display="'587-2990-6-ND" xr:uid="{A0F288D6-EDF1-41C5-A715-E84D14A054B5}"/>
+    <hyperlink ref="C22" r:id="rId10" tooltip="Supplier" display="'2019-RK73H2ATTD3300FCT-ND" xr:uid="{1C9997EC-2772-4E3A-9743-6787F0BFCF5D}"/>
+    <hyperlink ref="C23" r:id="rId11" tooltip="Supplier" display="'200-FSI11003GDAD" xr:uid="{58FE0FED-2B21-4A9C-89B3-33CB675E4B2E}"/>
+    <hyperlink ref="C24" r:id="rId12" tooltip="Supplier" display="'200-TSW10208GSRA" xr:uid="{AD0CD7AA-0B48-46C2-826B-B986A09C7CBD}"/>
+    <hyperlink ref="C25" r:id="rId13" tooltip="Supplier" display="'340-278808-TRAY" xr:uid="{0C6A265F-4BE4-47BB-83B5-CFAFAE704E54}"/>
+    <hyperlink ref="C26" r:id="rId14" tooltip="Supplier" display="'538-503182-1852" xr:uid="{298045F6-1219-4763-96E0-97D02BE97CE3}"/>
+    <hyperlink ref="E11" r:id="rId15" tooltip="Supplier" display="'71-CRCW0805-10K-E3" xr:uid="{F0931F1B-3E72-4FC2-AFAB-F99108874557}"/>
+    <hyperlink ref="E12" tooltip="Supplier" display="'" xr:uid="{AD33A1E5-DCC6-43D2-826A-5CA8086AF486}"/>
+    <hyperlink ref="E13" tooltip="Supplier" display="'" xr:uid="{B35B46C0-E4CF-471C-8F84-38E46A2E3DCB}"/>
+    <hyperlink ref="E14" r:id="rId16" tooltip="Supplier" display="'603-RC0805JR-070RL" xr:uid="{BDD9C457-49DF-4587-BBD4-9D48E1E26032}"/>
+    <hyperlink ref="E15" r:id="rId17" tooltip="Supplier" display="'SAM1039-03-ND" xr:uid="{593CD946-9940-491F-93C2-20F2A08848B7}"/>
+    <hyperlink ref="E16" r:id="rId18" tooltip="Supplier" display="'859-LTST-C170KFKT" xr:uid="{C73468A2-0BC2-4E2F-81C5-AFC4B951F218}"/>
+    <hyperlink ref="E17" r:id="rId19" tooltip="Supplier" display="'595-SN74LVC125APWR" xr:uid="{C91CD228-58ED-4440-BB04-72B74874F1B2}"/>
+    <hyperlink ref="E18" r:id="rId20" tooltip="Supplier" display="'603-RC0805FR-07100KL" xr:uid="{52B0EF20-4AA8-4BC9-A154-AD75298AF6E0}"/>
+    <hyperlink ref="E19" r:id="rId21" tooltip="Supplier" display="'603-CC805KRX7R8BB104" xr:uid="{C8647658-00BC-42C4-89F5-E74BFCF2F424}"/>
+    <hyperlink ref="E20" r:id="rId22" tooltip="Supplier" display="'603-CC201KRX7R9BB101" xr:uid="{84C4922D-B8B2-4244-87E0-FEC1891E09B6}"/>
+    <hyperlink ref="E21" r:id="rId23" tooltip="Supplier" display="'963-TMK212AB7475KG-T" xr:uid="{2B4DDDCD-8552-493F-A7D5-83009AC6E596}"/>
+    <hyperlink ref="E22" r:id="rId24" tooltip="Supplier" display="'660-RK73H2ATTD3300F" xr:uid="{3B900500-BA0C-4A69-9163-966D244697EB}"/>
+    <hyperlink ref="E23" r:id="rId25" tooltip="Supplier" display="'SAM9412-ND" xr:uid="{966D1164-D175-4B0D-8DF9-68079AE6CF83}"/>
+    <hyperlink ref="E24" r:id="rId26" tooltip="Supplier" display="'SAM1039-02-ND" xr:uid="{F904A4F0-64E0-43CE-9788-711B518ADDCC}"/>
+    <hyperlink ref="E25" r:id="rId27" tooltip="Supplier" display="'557-1789-ND" xr:uid="{CBD8AEFB-0B6D-45FF-BE08-A0A07F0020FB}"/>
+    <hyperlink ref="E26" r:id="rId28" tooltip="Supplier" display="'WM12834CT-ND" xr:uid="{203FC55D-4652-4207-9730-61278EF83FF0}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId29"/>

</xml_diff>

<commit_message>
DB_Memory: doc: Updated output files and documentation with revision 1.2 closes #20
</commit_message>
<xml_diff>
--- a/Memory_Expansion_Daughter_Board/hardware/Output_files/Bill of Materials/Bill of Materials-DB_Memory.xlsx
+++ b/Memory_Expansion_Daughter_Board/hardware/Output_files/Bill of Materials/Bill of Materials-DB_Memory.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B074A4F-AD01-4C72-9C6D-F0583FEA357B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8A59DBD-95A4-4D5F-B525-5C0F0B4C29A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="1605" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25845" yWindow="-675" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -67,10 +67,10 @@
     <t>&lt;Parameter ProductCode not found&gt;</t>
   </si>
   <si>
-    <t>24/03/2020</t>
-  </si>
-  <si>
-    <t>11:18:38</t>
+    <t>20/04/2020</t>
+  </si>
+  <si>
+    <t>17:19:00</t>
   </si>
   <si>
     <t>Supplier 1</t>
@@ -316,7 +316,7 @@
     <t>Designator</t>
   </si>
   <si>
-    <t>R2, R3, R4, R5, R7, R8, R9, R10, R11, R12, R13, R14, R15</t>
+    <t>R2, R3, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15</t>
   </si>
   <si>
     <t>M1, M2, M3, M4</t>
@@ -328,37 +328,37 @@
     <t>J_V1, J_V2, J_V3</t>
   </si>
   <si>
-    <t>P2, P3</t>
+    <t>P3, P4</t>
   </si>
   <si>
     <t>D1</t>
   </si>
   <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
     <t>U2</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>U1</t>
   </si>
   <si>
     <t>SC1</t>
@@ -1265,11 +1265,11 @@
       </c>
       <c r="G8" s="15">
         <f ca="1">TODAY()</f>
-        <v>43914</v>
+        <v>43941</v>
       </c>
       <c r="H8" s="16">
         <f ca="1">NOW()</f>
-        <v>43914.471456712963</v>
+        <v>43941.721688310186</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
@@ -2104,38 +2104,38 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" tooltip="Supplier" display="'541-10.0KCCT-ND" xr:uid="{EDD08F27-801C-46DA-8E9F-C88562AF06A0}"/>
-    <hyperlink ref="C12" tooltip="Supplier" display="'" xr:uid="{390C8A83-7557-43B3-8AF5-B4D02F0E7959}"/>
-    <hyperlink ref="C13" tooltip="Supplier" display="'" xr:uid="{C5523B0D-FD17-4283-A930-B677E2FE27ED}"/>
-    <hyperlink ref="C14" r:id="rId2" tooltip="Supplier" display="'311-0.0ARCT-ND" xr:uid="{7F3F3DB4-E824-4A2C-A891-52D00F4D7ACC}"/>
-    <hyperlink ref="C15" r:id="rId3" tooltip="Supplier" display="'200-TSW10308GSRA" xr:uid="{D7A61844-0204-42C8-91B5-D5F4C3CEC40E}"/>
-    <hyperlink ref="C16" r:id="rId4" tooltip="Supplier" display="'160-1413-1-ND" xr:uid="{AC6E6377-A61E-4DD5-B45A-B8CE4BCD27DD}"/>
-    <hyperlink ref="C17" r:id="rId5" tooltip="Supplier" display="'296-1222-1-ND" xr:uid="{6CBB4872-E5BA-4F10-B373-DE1DB3D918A4}"/>
-    <hyperlink ref="C18" r:id="rId6" tooltip="Supplier" display="'311-100KCRCT-ND" xr:uid="{70AFAAAD-37F8-475F-8E70-BDF4AB2D6FDA}"/>
-    <hyperlink ref="C19" r:id="rId7" tooltip="Supplier" display="'311-1141-1-ND" xr:uid="{E5CC9A02-8005-4EB3-9174-4019B579B0DA}"/>
-    <hyperlink ref="C20" r:id="rId8" tooltip="Supplier" display="'311-1401-1-ND" xr:uid="{0B343FEF-8427-483E-B423-D63E825B98CE}"/>
-    <hyperlink ref="C21" r:id="rId9" tooltip="Supplier" display="'587-2990-6-ND" xr:uid="{A0F288D6-EDF1-41C5-A715-E84D14A054B5}"/>
-    <hyperlink ref="C22" r:id="rId10" tooltip="Supplier" display="'2019-RK73H2ATTD3300FCT-ND" xr:uid="{1C9997EC-2772-4E3A-9743-6787F0BFCF5D}"/>
-    <hyperlink ref="C23" r:id="rId11" tooltip="Supplier" display="'200-FSI11003GDAD" xr:uid="{58FE0FED-2B21-4A9C-89B3-33CB675E4B2E}"/>
-    <hyperlink ref="C24" r:id="rId12" tooltip="Supplier" display="'200-TSW10208GSRA" xr:uid="{AD0CD7AA-0B48-46C2-826B-B986A09C7CBD}"/>
-    <hyperlink ref="C25" r:id="rId13" tooltip="Supplier" display="'340-278808-TRAY" xr:uid="{0C6A265F-4BE4-47BB-83B5-CFAFAE704E54}"/>
-    <hyperlink ref="C26" r:id="rId14" tooltip="Supplier" display="'538-503182-1852" xr:uid="{298045F6-1219-4763-96E0-97D02BE97CE3}"/>
-    <hyperlink ref="E11" r:id="rId15" tooltip="Supplier" display="'71-CRCW0805-10K-E3" xr:uid="{F0931F1B-3E72-4FC2-AFAB-F99108874557}"/>
-    <hyperlink ref="E12" tooltip="Supplier" display="'" xr:uid="{AD33A1E5-DCC6-43D2-826A-5CA8086AF486}"/>
-    <hyperlink ref="E13" tooltip="Supplier" display="'" xr:uid="{B35B46C0-E4CF-471C-8F84-38E46A2E3DCB}"/>
-    <hyperlink ref="E14" r:id="rId16" tooltip="Supplier" display="'603-RC0805JR-070RL" xr:uid="{BDD9C457-49DF-4587-BBD4-9D48E1E26032}"/>
-    <hyperlink ref="E15" r:id="rId17" tooltip="Supplier" display="'SAM1039-03-ND" xr:uid="{593CD946-9940-491F-93C2-20F2A08848B7}"/>
-    <hyperlink ref="E16" r:id="rId18" tooltip="Supplier" display="'859-LTST-C170KFKT" xr:uid="{C73468A2-0BC2-4E2F-81C5-AFC4B951F218}"/>
-    <hyperlink ref="E17" r:id="rId19" tooltip="Supplier" display="'595-SN74LVC125APWR" xr:uid="{C91CD228-58ED-4440-BB04-72B74874F1B2}"/>
-    <hyperlink ref="E18" r:id="rId20" tooltip="Supplier" display="'603-RC0805FR-07100KL" xr:uid="{52B0EF20-4AA8-4BC9-A154-AD75298AF6E0}"/>
-    <hyperlink ref="E19" r:id="rId21" tooltip="Supplier" display="'603-CC805KRX7R8BB104" xr:uid="{C8647658-00BC-42C4-89F5-E74BFCF2F424}"/>
-    <hyperlink ref="E20" r:id="rId22" tooltip="Supplier" display="'603-CC201KRX7R9BB101" xr:uid="{84C4922D-B8B2-4244-87E0-FEC1891E09B6}"/>
-    <hyperlink ref="E21" r:id="rId23" tooltip="Supplier" display="'963-TMK212AB7475KG-T" xr:uid="{2B4DDDCD-8552-493F-A7D5-83009AC6E596}"/>
-    <hyperlink ref="E22" r:id="rId24" tooltip="Supplier" display="'660-RK73H2ATTD3300F" xr:uid="{3B900500-BA0C-4A69-9163-966D244697EB}"/>
-    <hyperlink ref="E23" r:id="rId25" tooltip="Supplier" display="'SAM9412-ND" xr:uid="{966D1164-D175-4B0D-8DF9-68079AE6CF83}"/>
-    <hyperlink ref="E24" r:id="rId26" tooltip="Supplier" display="'SAM1039-02-ND" xr:uid="{F904A4F0-64E0-43CE-9788-711B518ADDCC}"/>
-    <hyperlink ref="E25" r:id="rId27" tooltip="Supplier" display="'557-1789-ND" xr:uid="{CBD8AEFB-0B6D-45FF-BE08-A0A07F0020FB}"/>
-    <hyperlink ref="E26" r:id="rId28" tooltip="Supplier" display="'WM12834CT-ND" xr:uid="{203FC55D-4652-4207-9730-61278EF83FF0}"/>
+    <hyperlink ref="C11" r:id="rId1" tooltip="Supplier" display="'541-10.0KCCT-ND" xr:uid="{7B61F501-3D57-4854-B02B-3BD86103135C}"/>
+    <hyperlink ref="C12" tooltip="Supplier" display="'" xr:uid="{1ADAA20F-D3DE-4477-B9A2-0E9E14283924}"/>
+    <hyperlink ref="C13" tooltip="Supplier" display="'" xr:uid="{0E694BFF-21CB-4C87-820E-FA2998196194}"/>
+    <hyperlink ref="C14" r:id="rId2" tooltip="Supplier" display="'311-0.0ARCT-ND" xr:uid="{3692E9DD-461C-43E2-BDF8-1E0CC1374ADB}"/>
+    <hyperlink ref="C15" r:id="rId3" tooltip="Supplier" display="'200-TSW10308GSRA" xr:uid="{B0493737-AA5B-4816-8935-5E73DB5859D0}"/>
+    <hyperlink ref="C16" r:id="rId4" tooltip="Supplier" display="'160-1413-1-ND" xr:uid="{7FD89C36-E81C-4B76-833A-D6801A284CB5}"/>
+    <hyperlink ref="C17" r:id="rId5" tooltip="Supplier" display="'296-1222-1-ND" xr:uid="{B3FDBC0B-0CD4-4742-8FFF-4874FF17E482}"/>
+    <hyperlink ref="C18" r:id="rId6" tooltip="Supplier" display="'311-100KCRCT-ND" xr:uid="{47775A2E-5B4C-491F-AA0C-C11D48E51E8E}"/>
+    <hyperlink ref="C19" r:id="rId7" tooltip="Supplier" display="'311-1141-1-ND" xr:uid="{8894F2E4-BA82-4BF9-BA23-8D1A1C723F69}"/>
+    <hyperlink ref="C20" r:id="rId8" tooltip="Supplier" display="'311-1401-1-ND" xr:uid="{76ED1FF8-BD82-4C91-B11C-3B3CD6DA8338}"/>
+    <hyperlink ref="C21" r:id="rId9" tooltip="Supplier" display="'587-2990-6-ND" xr:uid="{0136FD29-E3BA-4E57-AD2D-9640C10030FC}"/>
+    <hyperlink ref="C22" r:id="rId10" tooltip="Supplier" display="'2019-RK73H2ATTD3300FCT-ND" xr:uid="{CE0100D3-8421-4721-9EC7-4F0C121840AD}"/>
+    <hyperlink ref="C23" r:id="rId11" tooltip="Supplier" display="'200-FSI11003GDAD" xr:uid="{3B7014EC-3AFF-4902-85DE-7C7E5F687DDC}"/>
+    <hyperlink ref="C24" r:id="rId12" tooltip="Supplier" display="'200-TSW10208GSRA" xr:uid="{3A5B6944-4BA3-4865-A0EE-4267417A565C}"/>
+    <hyperlink ref="C25" r:id="rId13" tooltip="Supplier" display="'340-278808-TRAY" xr:uid="{DB2080D2-454C-476E-BB1C-9335F67D7750}"/>
+    <hyperlink ref="C26" r:id="rId14" tooltip="Supplier" display="'538-503182-1852" xr:uid="{734E8280-BBAB-4CBF-9208-38C6AB17E9DD}"/>
+    <hyperlink ref="E11" r:id="rId15" tooltip="Supplier" display="'71-CRCW0805-10K-E3" xr:uid="{521F7390-20BB-40E2-9CDE-43EA67D31BF7}"/>
+    <hyperlink ref="E12" tooltip="Supplier" display="'" xr:uid="{BBE6C2EF-F652-47A6-856B-365757C811E6}"/>
+    <hyperlink ref="E13" tooltip="Supplier" display="'" xr:uid="{E89427A7-9BCB-4EC1-85FC-BC3626AA06E7}"/>
+    <hyperlink ref="E14" r:id="rId16" tooltip="Supplier" display="'603-RC0805JR-070RL" xr:uid="{25DCEB33-E90D-47DB-B796-4CBAE8AA3278}"/>
+    <hyperlink ref="E15" r:id="rId17" tooltip="Supplier" display="'SAM1039-03-ND" xr:uid="{4174A873-193B-4420-82E8-860CCCC3E930}"/>
+    <hyperlink ref="E16" r:id="rId18" tooltip="Supplier" display="'859-LTST-C170KFKT" xr:uid="{F016BC75-148B-417A-AA31-1E4E1A58A7D9}"/>
+    <hyperlink ref="E17" r:id="rId19" tooltip="Supplier" display="'595-SN74LVC125APWR" xr:uid="{E07DD644-F021-4BE6-9D59-1BBE18782C65}"/>
+    <hyperlink ref="E18" r:id="rId20" tooltip="Supplier" display="'603-RC0805FR-07100KL" xr:uid="{C8147B50-33CA-4229-BF18-A3F60AEB5CFB}"/>
+    <hyperlink ref="E19" r:id="rId21" tooltip="Supplier" display="'603-CC805KRX7R8BB104" xr:uid="{EBF0C048-DCF2-4AF7-A4C8-AA95F5FC3042}"/>
+    <hyperlink ref="E20" r:id="rId22" tooltip="Supplier" display="'603-CC201KRX7R9BB101" xr:uid="{3EBC89AF-149A-430E-B213-CDF054C3FA4C}"/>
+    <hyperlink ref="E21" r:id="rId23" tooltip="Supplier" display="'963-TMK212AB7475KG-T" xr:uid="{B32AFE36-2CDD-42D5-8F3E-9D10827E79CF}"/>
+    <hyperlink ref="E22" r:id="rId24" tooltip="Supplier" display="'660-RK73H2ATTD3300F" xr:uid="{08A8F2E6-221A-4E28-A779-4EA5B26B49A4}"/>
+    <hyperlink ref="E23" r:id="rId25" tooltip="Supplier" display="'SAM9412-ND" xr:uid="{10B28EB2-DD71-4DBC-A601-0539B31C7CD6}"/>
+    <hyperlink ref="E24" r:id="rId26" tooltip="Supplier" display="'SAM1039-02-ND" xr:uid="{142E40E8-3658-4DE6-83E7-BD136E1F70D8}"/>
+    <hyperlink ref="E25" r:id="rId27" tooltip="Supplier" display="'557-1789-ND" xr:uid="{36696904-68DF-46F3-AFCA-1B001058F46D}"/>
+    <hyperlink ref="E26" r:id="rId28" tooltip="Supplier" display="'WM12834CT-ND" xr:uid="{6039AD70-2B49-47D4-BE87-613B1EE12C4D}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId29"/>

</xml_diff>

<commit_message>
DB_Memory: Updating output files for project revision 1.3
</commit_message>
<xml_diff>
--- a/Memory_Expansion_Daughter_Board/hardware/Output_files/Bill of Materials/Bill of Materials-DB_Memory.xlsx
+++ b/Memory_Expansion_Daughter_Board/hardware/Output_files/Bill of Materials/Bill of Materials-DB_Memory.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8A59DBD-95A4-4D5F-B525-5C0F0B4C29A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E455F5B-1E3D-4B62-A345-BC301EB92884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25845" yWindow="-675" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3060" yWindow="2970" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase" localSheetId="0" hidden="1">Plan1!$B$10:$K$10</definedName>
-    <definedName name="Print_Area" localSheetId="0">Plan1!$A$1:$K$26</definedName>
+    <definedName name="Print_Area" localSheetId="0">Plan1!$A$1:$K$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
   <si>
     <t>Source Data From:</t>
   </si>
@@ -67,10 +67,10 @@
     <t>&lt;Parameter ProductCode not found&gt;</t>
   </si>
   <si>
-    <t>20/04/2020</t>
-  </si>
-  <si>
-    <t>17:19:00</t>
+    <t>07/05/2020</t>
+  </si>
+  <si>
+    <t>11:25:48</t>
   </si>
   <si>
     <t>Supplier 1</t>
@@ -79,9 +79,6 @@
     <t>Digi-Key</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
@@ -214,12 +211,6 @@
     <t>10k</t>
   </si>
   <si>
-    <t>DB Mechanical Hole</t>
-  </si>
-  <si>
-    <t>Fiducial</t>
-  </si>
-  <si>
     <t>0R</t>
   </si>
   <si>
@@ -265,12 +256,6 @@
     <t>RES 10K OHM 1/8W 1%  0805</t>
   </si>
   <si>
-    <t>Mechanical Hole for DB board variants</t>
-  </si>
-  <si>
-    <t>Fiducial for DB board variants</t>
-  </si>
-  <si>
     <t>RES 0R OHM 1/8W JUMPER 0805</t>
   </si>
   <si>
@@ -317,12 +302,6 @@
   </si>
   <si>
     <t>R2, R3, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15</t>
-  </si>
-  <si>
-    <t>M1, M2, M3, M4</t>
-  </si>
-  <si>
-    <t>FD1, FD2, FD3</t>
   </si>
   <si>
     <t>J_V1, J_V2, J_V3</t>
@@ -664,21 +643,7 @@
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -1104,7 +1069,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
@@ -1265,11 +1230,11 @@
       </c>
       <c r="G8" s="15">
         <f ca="1">TODAY()</f>
-        <v>43941</v>
+        <v>43958</v>
       </c>
       <c r="H8" s="16">
         <f ca="1">NOW()</f>
-        <v>43941.721688310186</v>
+        <v>43958.476506597224</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
@@ -1300,31 +1265,31 @@
         <v>13</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>33</v>
-      </c>
       <c r="F10" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="L10" s="22"/>
     </row>
@@ -1337,66 +1302,66 @@
         <v>14</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I11" s="24">
         <v>13</v>
       </c>
       <c r="J11" s="34" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="23">
-        <f t="shared" ref="A12:A26" si="0">ROW(A12) - ROW($A$10)</f>
+        <f t="shared" ref="A12:A24" si="0">ROW(A12) - ROW($A$10)</f>
         <v>2</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D12" s="34" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H12" s="34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I12" s="24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12" s="34" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="K12" s="24"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="23">
         <f>ROW(A13) - ROW($A$10)</f>
         <v>3</v>
@@ -1405,32 +1370,32 @@
         <v>15</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I13" s="24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="K13" s="24"/>
     </row>
-    <row r="14" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="23">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1439,62 +1404,62 @@
         <v>14</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I14" s="24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J14" s="34" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="K14" s="24"/>
     </row>
-    <row r="15" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="23">
         <f>ROW(A15) - ROW($A$10)</f>
         <v>5</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I15" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15" s="34" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="K15" s="24"/>
     </row>
@@ -1507,28 +1472,28 @@
         <v>14</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I16" s="24">
         <v>1</v>
       </c>
       <c r="J16" s="34" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K16" s="24"/>
     </row>
@@ -1541,28 +1506,28 @@
         <v>14</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F17" s="34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H17" s="34" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I17" s="24">
         <v>1</v>
       </c>
       <c r="J17" s="34" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K17" s="24"/>
     </row>
@@ -1575,28 +1540,28 @@
         <v>14</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H18" s="34" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I18" s="24">
         <v>1</v>
       </c>
       <c r="J18" s="34" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="K18" s="24"/>
     </row>
@@ -1609,28 +1574,28 @@
         <v>14</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19" s="34" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G19" s="34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H19" s="34" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I19" s="24">
         <v>1</v>
       </c>
       <c r="J19" s="34" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K19" s="24"/>
     </row>
@@ -1643,28 +1608,28 @@
         <v>14</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H20" s="34" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I20" s="24">
         <v>1</v>
       </c>
       <c r="J20" s="34" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="K20" s="24"/>
     </row>
@@ -1674,203 +1639,151 @@
         <v>11</v>
       </c>
       <c r="B21" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>16</v>
-      </c>
       <c r="E21" s="35" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H21" s="34" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I21" s="24">
         <v>1</v>
       </c>
       <c r="J21" s="34" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="K21" s="24"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A22" s="23">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B22" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>16</v>
-      </c>
       <c r="E22" s="35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F22" s="34" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H22" s="34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I22" s="24">
         <v>1</v>
       </c>
       <c r="J22" s="34" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A23" s="23">
         <f>ROW(A23) - ROW($A$10)</f>
         <v>13</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D23" s="34" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G23" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H23" s="34" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I23" s="24">
         <v>1</v>
       </c>
       <c r="J23" s="34" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K23" s="24"/>
     </row>
-    <row r="24" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A24" s="23">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>14</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G24" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H24" s="34" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I24" s="24">
         <v>1</v>
       </c>
       <c r="J24" s="34" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K24" s="24"/>
     </row>
-    <row r="25" spans="1:11" ht="51" x14ac:dyDescent="0.25">
-      <c r="A25" s="23">
-        <f>ROW(A25) - ROW($A$10)</f>
-        <v>15</v>
-      </c>
-      <c r="B25" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="H25" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="I25" s="24">
-        <v>1</v>
-      </c>
-      <c r="J25" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="K25" s="24"/>
-    </row>
-    <row r="26" spans="1:11" ht="51" x14ac:dyDescent="0.25">
-      <c r="A26" s="23">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B26" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G26" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="H26" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="I26" s="24">
-        <v>1</v>
-      </c>
-      <c r="J26" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="K26" s="24"/>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F27" s="25"/>
@@ -1905,7 +1818,6 @@
       <c r="K30" s="25"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F31" s="25"/>
       <c r="G31" s="25"/>
       <c r="H31" s="25"/>
       <c r="I31" s="25"/>
@@ -1913,7 +1825,6 @@
       <c r="K31" s="25"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F32" s="25"/>
       <c r="G32" s="25"/>
       <c r="H32" s="25"/>
       <c r="I32" s="25"/>
@@ -2003,20 +1914,6 @@
       <c r="I44" s="25"/>
       <c r="J44" s="25"/>
       <c r="K44" s="25"/>
-    </row>
-    <row r="45" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
-    </row>
-    <row r="46" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="B10:K10" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -2029,113 +1926,99 @@
     <mergeCell ref="G5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="K11:K12">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"Not Fitted"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"Not Fitted"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" tooltip="Supplier" display="'541-10.0KCCT-ND" xr:uid="{7B61F501-3D57-4854-B02B-3BD86103135C}"/>
-    <hyperlink ref="C12" tooltip="Supplier" display="'" xr:uid="{1ADAA20F-D3DE-4477-B9A2-0E9E14283924}"/>
-    <hyperlink ref="C13" tooltip="Supplier" display="'" xr:uid="{0E694BFF-21CB-4C87-820E-FA2998196194}"/>
-    <hyperlink ref="C14" r:id="rId2" tooltip="Supplier" display="'311-0.0ARCT-ND" xr:uid="{3692E9DD-461C-43E2-BDF8-1E0CC1374ADB}"/>
-    <hyperlink ref="C15" r:id="rId3" tooltip="Supplier" display="'200-TSW10308GSRA" xr:uid="{B0493737-AA5B-4816-8935-5E73DB5859D0}"/>
-    <hyperlink ref="C16" r:id="rId4" tooltip="Supplier" display="'160-1413-1-ND" xr:uid="{7FD89C36-E81C-4B76-833A-D6801A284CB5}"/>
-    <hyperlink ref="C17" r:id="rId5" tooltip="Supplier" display="'296-1222-1-ND" xr:uid="{B3FDBC0B-0CD4-4742-8FFF-4874FF17E482}"/>
-    <hyperlink ref="C18" r:id="rId6" tooltip="Supplier" display="'311-100KCRCT-ND" xr:uid="{47775A2E-5B4C-491F-AA0C-C11D48E51E8E}"/>
-    <hyperlink ref="C19" r:id="rId7" tooltip="Supplier" display="'311-1141-1-ND" xr:uid="{8894F2E4-BA82-4BF9-BA23-8D1A1C723F69}"/>
-    <hyperlink ref="C20" r:id="rId8" tooltip="Supplier" display="'311-1401-1-ND" xr:uid="{76ED1FF8-BD82-4C91-B11C-3B3CD6DA8338}"/>
-    <hyperlink ref="C21" r:id="rId9" tooltip="Supplier" display="'587-2990-6-ND" xr:uid="{0136FD29-E3BA-4E57-AD2D-9640C10030FC}"/>
-    <hyperlink ref="C22" r:id="rId10" tooltip="Supplier" display="'2019-RK73H2ATTD3300FCT-ND" xr:uid="{CE0100D3-8421-4721-9EC7-4F0C121840AD}"/>
-    <hyperlink ref="C23" r:id="rId11" tooltip="Supplier" display="'200-FSI11003GDAD" xr:uid="{3B7014EC-3AFF-4902-85DE-7C7E5F687DDC}"/>
-    <hyperlink ref="C24" r:id="rId12" tooltip="Supplier" display="'200-TSW10208GSRA" xr:uid="{3A5B6944-4BA3-4865-A0EE-4267417A565C}"/>
-    <hyperlink ref="C25" r:id="rId13" tooltip="Supplier" display="'340-278808-TRAY" xr:uid="{DB2080D2-454C-476E-BB1C-9335F67D7750}"/>
-    <hyperlink ref="C26" r:id="rId14" tooltip="Supplier" display="'538-503182-1852" xr:uid="{734E8280-BBAB-4CBF-9208-38C6AB17E9DD}"/>
-    <hyperlink ref="E11" r:id="rId15" tooltip="Supplier" display="'71-CRCW0805-10K-E3" xr:uid="{521F7390-20BB-40E2-9CDE-43EA67D31BF7}"/>
-    <hyperlink ref="E12" tooltip="Supplier" display="'" xr:uid="{BBE6C2EF-F652-47A6-856B-365757C811E6}"/>
-    <hyperlink ref="E13" tooltip="Supplier" display="'" xr:uid="{E89427A7-9BCB-4EC1-85FC-BC3626AA06E7}"/>
-    <hyperlink ref="E14" r:id="rId16" tooltip="Supplier" display="'603-RC0805JR-070RL" xr:uid="{25DCEB33-E90D-47DB-B796-4CBAE8AA3278}"/>
-    <hyperlink ref="E15" r:id="rId17" tooltip="Supplier" display="'SAM1039-03-ND" xr:uid="{4174A873-193B-4420-82E8-860CCCC3E930}"/>
-    <hyperlink ref="E16" r:id="rId18" tooltip="Supplier" display="'859-LTST-C170KFKT" xr:uid="{F016BC75-148B-417A-AA31-1E4E1A58A7D9}"/>
-    <hyperlink ref="E17" r:id="rId19" tooltip="Supplier" display="'595-SN74LVC125APWR" xr:uid="{E07DD644-F021-4BE6-9D59-1BBE18782C65}"/>
-    <hyperlink ref="E18" r:id="rId20" tooltip="Supplier" display="'603-RC0805FR-07100KL" xr:uid="{C8147B50-33CA-4229-BF18-A3F60AEB5CFB}"/>
-    <hyperlink ref="E19" r:id="rId21" tooltip="Supplier" display="'603-CC805KRX7R8BB104" xr:uid="{EBF0C048-DCF2-4AF7-A4C8-AA95F5FC3042}"/>
-    <hyperlink ref="E20" r:id="rId22" tooltip="Supplier" display="'603-CC201KRX7R9BB101" xr:uid="{3EBC89AF-149A-430E-B213-CDF054C3FA4C}"/>
-    <hyperlink ref="E21" r:id="rId23" tooltip="Supplier" display="'963-TMK212AB7475KG-T" xr:uid="{B32AFE36-2CDD-42D5-8F3E-9D10827E79CF}"/>
-    <hyperlink ref="E22" r:id="rId24" tooltip="Supplier" display="'660-RK73H2ATTD3300F" xr:uid="{08A8F2E6-221A-4E28-A779-4EA5B26B49A4}"/>
-    <hyperlink ref="E23" r:id="rId25" tooltip="Supplier" display="'SAM9412-ND" xr:uid="{10B28EB2-DD71-4DBC-A601-0539B31C7CD6}"/>
-    <hyperlink ref="E24" r:id="rId26" tooltip="Supplier" display="'SAM1039-02-ND" xr:uid="{142E40E8-3658-4DE6-83E7-BD136E1F70D8}"/>
-    <hyperlink ref="E25" r:id="rId27" tooltip="Supplier" display="'557-1789-ND" xr:uid="{36696904-68DF-46F3-AFCA-1B001058F46D}"/>
-    <hyperlink ref="E26" r:id="rId28" tooltip="Supplier" display="'WM12834CT-ND" xr:uid="{6039AD70-2B49-47D4-BE87-613B1EE12C4D}"/>
+    <hyperlink ref="C11" r:id="rId1" tooltip="Supplier" display="'541-10.0KCCT-ND" xr:uid="{17E72478-80CE-43B5-9DDE-142443A58E22}"/>
+    <hyperlink ref="C12" r:id="rId2" tooltip="Supplier" display="'311-0.0ARCT-ND" xr:uid="{E2F8764E-FAF9-4EDF-9B96-418088E33A5C}"/>
+    <hyperlink ref="C13" r:id="rId3" tooltip="Supplier" display="'200-TSW10308GSRA" xr:uid="{164FF67D-5537-41B8-8B4C-0B9229D0D965}"/>
+    <hyperlink ref="C14" r:id="rId4" tooltip="Supplier" display="'160-1413-1-ND" xr:uid="{84E57943-6F03-48DB-AA75-11EE818D6E8D}"/>
+    <hyperlink ref="C15" r:id="rId5" tooltip="Supplier" display="'296-1222-1-ND" xr:uid="{7593BEDE-FEF5-4AD3-A0E2-A1E373174569}"/>
+    <hyperlink ref="C16" r:id="rId6" tooltip="Supplier" display="'311-100KCRCT-ND" xr:uid="{33EEE828-B994-400A-B364-8A00AEBF797B}"/>
+    <hyperlink ref="C17" r:id="rId7" tooltip="Supplier" display="'311-1141-1-ND" xr:uid="{5E730497-B85F-40FF-B6EB-E6116A1012D3}"/>
+    <hyperlink ref="C18" r:id="rId8" tooltip="Supplier" display="'311-1401-1-ND" xr:uid="{DAD61141-1844-4B83-98D2-9062FEC0828A}"/>
+    <hyperlink ref="C19" r:id="rId9" tooltip="Supplier" display="'587-2990-6-ND" xr:uid="{78196734-F261-4C74-B854-7E32F3D31ED2}"/>
+    <hyperlink ref="C20" r:id="rId10" tooltip="Supplier" display="'2019-RK73H2ATTD3300FCT-ND" xr:uid="{8498A9C3-086A-4AE0-BD53-76B618641952}"/>
+    <hyperlink ref="C21" r:id="rId11" tooltip="Supplier" display="'200-FSI11003GDAD" xr:uid="{66B4AC6D-DF5A-4E87-BF1A-CCB58B245A9D}"/>
+    <hyperlink ref="C22" r:id="rId12" tooltip="Supplier" display="'200-TSW10208GSRA" xr:uid="{DF62A931-E801-4573-92AC-3E272A8C1342}"/>
+    <hyperlink ref="C23" r:id="rId13" tooltip="Supplier" display="'340-278808-TRAY" xr:uid="{ED70A30D-AB86-4F22-982F-7AA92CA12646}"/>
+    <hyperlink ref="C24" r:id="rId14" tooltip="Supplier" display="'538-503182-1852" xr:uid="{4E5671C5-7596-4B94-82C6-E263A69B9FE2}"/>
+    <hyperlink ref="E11" r:id="rId15" tooltip="Supplier" display="'71-CRCW0805-10K-E3" xr:uid="{712F374E-F8DA-4792-AB5A-2D91B0C7F9C5}"/>
+    <hyperlink ref="E12" r:id="rId16" tooltip="Supplier" display="'603-RC0805JR-070RL" xr:uid="{C7DF561D-568D-4AB5-90CB-FC0D1871E52B}"/>
+    <hyperlink ref="E13" r:id="rId17" tooltip="Supplier" display="'SAM1039-03-ND" xr:uid="{D909EADD-F899-4C2F-9E80-5FD948A1ACE1}"/>
+    <hyperlink ref="E14" r:id="rId18" tooltip="Supplier" display="'859-LTST-C170KFKT" xr:uid="{ACCC3341-828F-4302-BC49-BF47481B71EF}"/>
+    <hyperlink ref="E15" r:id="rId19" tooltip="Supplier" display="'595-SN74LVC125APWR" xr:uid="{45839448-6403-4FE6-9A59-56F081665590}"/>
+    <hyperlink ref="E16" r:id="rId20" tooltip="Supplier" display="'603-RC0805FR-07100KL" xr:uid="{1A3030DD-F22A-4CAA-87CA-151FBC57FBD6}"/>
+    <hyperlink ref="E17" r:id="rId21" tooltip="Supplier" display="'603-CC805KRX7R8BB104" xr:uid="{34C35743-D3B2-445F-9637-F5B2B0406846}"/>
+    <hyperlink ref="E18" r:id="rId22" tooltip="Supplier" display="'603-CC201KRX7R9BB101" xr:uid="{C0814BDF-3F6A-4BDC-9F39-A989B1C8A653}"/>
+    <hyperlink ref="E19" r:id="rId23" tooltip="Supplier" display="'963-TMK212AB7475KG-T" xr:uid="{AEBC398D-785B-491A-B420-7BB3D3F03959}"/>
+    <hyperlink ref="E20" r:id="rId24" tooltip="Supplier" display="'660-RK73H2ATTD3300F" xr:uid="{00571C42-9C05-44C8-8B32-C472E04AE9D6}"/>
+    <hyperlink ref="E21" r:id="rId25" tooltip="Supplier" display="'SAM9412-ND" xr:uid="{72BB9F61-D5A3-49E7-B5EA-113337A85102}"/>
+    <hyperlink ref="E22" r:id="rId26" tooltip="Supplier" display="'SAM1039-02-ND" xr:uid="{2A07C911-A085-4C47-AE8F-E340DBE98B83}"/>
+    <hyperlink ref="E23" r:id="rId27" tooltip="Supplier" display="'557-1789-ND" xr:uid="{D121EB02-630C-4537-AE85-6C8A13D29ABF}"/>
+    <hyperlink ref="E24" r:id="rId28" tooltip="Supplier" display="'WM12834CT-ND" xr:uid="{675D7783-66F1-4AF9-95FA-DEA1D1FB5268}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId29"/>

</xml_diff>